<commit_message>
Added XNA tutorial. XNA can now interface with the Emotiv Headset and changes screens based on input.
</commit_message>
<xml_diff>
--- a/Documents/Logs/TimeLog_EricCarlson.xlsx
+++ b/Documents/Logs/TimeLog_EricCarlson.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="26">
   <si>
     <t>Monday</t>
   </si>
@@ -101,6 +101,15 @@
   </si>
   <si>
     <t>Log Updates</t>
+  </si>
+  <si>
+    <t>XNA Tutorial</t>
+  </si>
+  <si>
+    <t>Re-install</t>
+  </si>
+  <si>
+    <t>XNA Research/Interfacing with Emotiv</t>
   </si>
 </sst>
 </file>
@@ -173,13 +182,13 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -467,7 +476,7 @@
   <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+      <selection activeCell="C47" sqref="A47:C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -621,11 +630,11 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
       <c r="D14">
         <f>SUM(D10:D13)</f>
         <v>6.25</v>
@@ -679,11 +688,11 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
       <c r="D20">
         <f>SUM(D18:D19)</f>
         <v>3</v>
@@ -737,11 +746,11 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
       <c r="D26">
         <f>SUM(D24:D25)</f>
         <v>8</v>
@@ -795,11 +804,11 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
       <c r="D32">
         <f>SUM(D30:D31)</f>
         <v>3</v>
@@ -844,23 +853,22 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
       <c r="D47">
         <f>SUM(D3,D4,D5,D10,D11,D12,D13,D18,D19,D24,D25,D30,D31)</f>
         <v>23.5</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A26:C26"/>
     <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A47:C47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -869,17 +877,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -907,7 +915,7 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="B3" s="1">
-        <v>6.25E-2</v>
+        <v>0.5625</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>
@@ -917,26 +925,70 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="9" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="2" t="s">
+      <c r="A4" s="1">
+        <v>0.5625</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>3</v>
+    <row r="9" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>0.5625</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11">
+        <v>1.5</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
@@ -958,47 +1010,104 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="2" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>3</v>
+    <row r="20" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23">
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -1017,7 +1126,7 @@
     </row>
     <row r="29" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -1034,7 +1143,82 @@
         <v>3</v>
       </c>
     </row>
+    <row r="33" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="B35" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0.125</v>
+      </c>
+      <c r="C36" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39">
+        <f>SUM(D37,D23,D17,D11,D6)</f>
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A37:C37"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Log and Research Update
</commit_message>
<xml_diff>
--- a/Documents/Logs/TimeLog_EricCarlson.xlsx
+++ b/Documents/Logs/TimeLog_EricCarlson.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcarlson\Documents\School\Quarter 7\Capstone\Eric Carlson - Mind Control\Documents\Time Logs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcarlson\Documents\School\Quarter 7\Capstone\Eric Carlson - Mind Control\Documents\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9972"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9972" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="27">
   <si>
     <t>Monday</t>
   </si>
@@ -98,6 +98,21 @@
   </si>
   <si>
     <t>This Week's Total Hours</t>
+  </si>
+  <si>
+    <t>Create/Load Profiles</t>
+  </si>
+  <si>
+    <t>Installing UI Controls</t>
+  </si>
+  <si>
+    <t>Research For UI Controls</t>
+  </si>
+  <si>
+    <t>Create/Load Profiles(Completed)</t>
+  </si>
+  <si>
+    <t>Project Management/Source Control</t>
   </si>
 </sst>
 </file>
@@ -165,11 +180,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -179,6 +197,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
@@ -463,7 +483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
@@ -618,11 +638,11 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
       <c r="D14">
         <f>SUM(D10:D13)</f>
         <v>6.25</v>
@@ -676,11 +696,11 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
       <c r="D20">
         <f>SUM(D18:D19)</f>
         <v>3</v>
@@ -734,11 +754,11 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
       <c r="D26">
         <f>SUM(D24:D25)</f>
         <v>8</v>
@@ -792,11 +812,11 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
       <c r="D32">
         <f>SUM(D30:D31)</f>
         <v>3</v>
@@ -841,11 +861,11 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
       <c r="D47">
         <f>SUM(D3:D5,D10,D11,D12,D13,D18,D19,D24,D25,D30,D31)</f>
         <v>23.5</v>
@@ -869,7 +889,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D26"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1028,26 +1048,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1061,58 +1081,113 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="2" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="8">
+        <v>2</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="8">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5">
+        <f>SUM(D3:D4)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="2" t="s">
+    <row r="8" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="8">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11">
+        <f>SUM(D9:D10)</f>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
@@ -1126,28 +1201,76 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>3</v>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="8">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="B17" s="1">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>6.25E-2</v>
+      </c>
+      <c r="B18" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19">
+        <f>SUM(D15:D18)</f>
+        <v>9.5</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -1164,9 +1287,21 @@
         <v>3</v>
       </c>
     </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="8">
+        <v>3</v>
+      </c>
+    </row>
     <row r="25" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -1183,7 +1318,60 @@
         <v>3</v>
       </c>
     </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="8"/>
+    </row>
+    <row r="29" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="9"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A19:C19"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added DigitalRune to the vendor folder.
</commit_message>
<xml_diff>
--- a/Documents/Logs/TimeLog_EricCarlson.xlsx
+++ b/Documents/Logs/TimeLog_EricCarlson.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="30">
   <si>
     <t>Monday</t>
   </si>
@@ -113,6 +113,15 @@
   </si>
   <si>
     <t>Project Management/Source Control</t>
+  </si>
+  <si>
+    <t>Create Main Menu flow</t>
+  </si>
+  <si>
+    <t>Setup the settings menu</t>
+  </si>
+  <si>
+    <t>Week 3 Total</t>
   </si>
 </sst>
 </file>
@@ -188,6 +197,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -197,8 +208,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
@@ -638,11 +647,11 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
       <c r="D14">
         <f>SUM(D10:D13)</f>
         <v>6.25</v>
@@ -696,11 +705,11 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
       <c r="D20">
         <f>SUM(D18:D19)</f>
         <v>3</v>
@@ -754,11 +763,11 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
       <c r="D26">
         <f>SUM(D24:D25)</f>
         <v>8</v>
@@ -812,11 +821,11 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
       <c r="D32">
         <f>SUM(D30:D31)</f>
         <v>3</v>
@@ -861,11 +870,11 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
       <c r="D47">
         <f>SUM(D3:D5,D10,D11,D12,D13,D18,D19,D24,D25,D30,D31)</f>
         <v>23.5</v>
@@ -1050,8 +1059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1089,11 +1098,11 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="8">
-        <v>2</v>
-      </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
+      <c r="D3" s="5">
+        <v>2</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1106,7 +1115,7 @@
       <c r="C4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="5">
         <v>2</v>
       </c>
       <c r="E4" s="1"/>
@@ -1114,11 +1123,11 @@
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
       <c r="D5">
         <f>SUM(D3:D4)</f>
         <v>4</v>
@@ -1153,7 +1162,7 @@
       <c r="C9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="5">
         <v>2.5</v>
       </c>
     </row>
@@ -1211,7 +1220,7 @@
       <c r="C15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="5">
         <v>2.5</v>
       </c>
     </row>
@@ -1258,11 +1267,11 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
       <c r="D19">
         <f>SUM(D15:D18)</f>
         <v>9.5</v>
@@ -1294,83 +1303,147 @@
       <c r="B23" s="1">
         <v>0.625</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="2" t="s">
+      <c r="C23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="8"/>
-    </row>
-    <row r="29" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="2" t="s">
+    <row r="28" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="5"/>
+    </row>
+    <row r="31" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="2" t="s">
+    <row r="32" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C33" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>3</v>
+    <row r="37" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40">
+        <f>SUM(D34,D25,D19,D11,D5)</f>
+        <v>26</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="9"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A40:C40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Created Contact Quality Images Created multi-purpose Contact Quality Panel
</commit_message>
<xml_diff>
--- a/Documents/Logs/TimeLog_EricCarlson.xlsx
+++ b/Documents/Logs/TimeLog_EricCarlson.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9972" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9972" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="36">
   <si>
     <t>Monday</t>
   </si>
@@ -122,6 +122,24 @@
   </si>
   <si>
     <t>Week 3 Total</t>
+  </si>
+  <si>
+    <t>Implementing Settings Menu</t>
+  </si>
+  <si>
+    <t>Training/Saving/Reading Cognitiv Actions</t>
+  </si>
+  <si>
+    <t>Creating Contact Quality Panel</t>
+  </si>
+  <si>
+    <t>Creating Contact Quality Images</t>
+  </si>
+  <si>
+    <t>Project Management/Source Control/Time Log</t>
+  </si>
+  <si>
+    <t>Positioning Contact Quality Images</t>
   </si>
 </sst>
 </file>
@@ -189,7 +207,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
@@ -206,6 +224,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1059,7 +1080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
@@ -1451,17 +1472,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D26"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1485,128 +1506,317 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="A3" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="2" t="s">
+      <c r="A4" s="1">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="2" t="s">
+    <row r="8" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="2" t="s">
+    <row r="15" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="2" t="s">
+    <row r="21" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>0</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="2" t="s">
+    <row r="30" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="2" t="s">
+    <row r="34" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="3" t="s">
+    <row r="38" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A18:C18"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Contact Quality is fully functional.
</commit_message>
<xml_diff>
--- a/Documents/Logs/TimeLog_EricCarlson.xlsx
+++ b/Documents/Logs/TimeLog_EricCarlson.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="38">
   <si>
     <t>Monday</t>
   </si>
@@ -140,6 +140,12 @@
   </si>
   <si>
     <t>Positioning Contact Quality Images</t>
+  </si>
+  <si>
+    <t>Updating Contact Quality Images</t>
+  </si>
+  <si>
+    <t>Week 4 Total</t>
   </si>
 </sst>
 </file>
@@ -1472,10 +1478,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1743,79 +1749,122 @@
         <v>34</v>
       </c>
       <c r="D25">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>4.1666666666666664E-2</v>
       </c>
+      <c r="B26" s="1">
+        <v>6.9444444444444434E-2</v>
+      </c>
       <c r="C26" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="2" t="s">
+      <c r="D26">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>6.9444444444444434E-2</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27">
+        <v>2.33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="2" t="s">
+    <row r="31" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="2" t="s">
+    <row r="35" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>3</v>
+    <row r="39" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42">
+        <f>SUM(D28,D18,D12,D5)</f>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A42:C42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Pause functionality for EEG abnormalities now completed Upon pause, program tells the user how to alleviate abnormalities
</commit_message>
<xml_diff>
--- a/Documents/Logs/TimeLog_EricCarlson.xlsx
+++ b/Documents/Logs/TimeLog_EricCarlson.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="38">
   <si>
     <t>Monday</t>
   </si>
@@ -145,7 +145,7 @@
     <t>Updating Contact Quality Images</t>
   </si>
   <si>
-    <t>Week 4 Total</t>
+    <t>Pause Functionality for EEG abnormalities</t>
   </si>
 </sst>
 </file>
@@ -1478,10 +1478,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1809,54 +1809,86 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="2" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="2" t="s">
+    <row r="36" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B37" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42">
-        <f>SUM(D28,D18,D12,D5)</f>
-        <v>30</v>
-      </c>
+    <row r="42" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1864,7 +1896,7 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A33:C33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Research on USB Relay
</commit_message>
<xml_diff>
--- a/Documents/Logs/TimeLog_EricCarlson.xlsx
+++ b/Documents/Logs/TimeLog_EricCarlson.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9972" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9972" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="39">
   <si>
     <t>Monday</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>Pause Functionality for EEG abnormalities</t>
+  </si>
+  <si>
+    <t>Research On USB Relay</t>
   </si>
 </sst>
 </file>
@@ -1480,7 +1483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
@@ -1904,17 +1907,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1938,128 +1941,161 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="A3" s="1">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="2" t="s">
+      <c r="A4" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="2" t="s">
+    <row r="8" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="2" t="s">
+    <row r="12" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="2" t="s">
+    <row r="16" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="2" t="s">
+    <row r="20" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="2" t="s">
+    <row r="24" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="3" t="s">
+    <row r="28" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A5:C5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
3D world completed. Need to implement it in the menu.
</commit_message>
<xml_diff>
--- a/Documents/Logs/TimeLog_EricCarlson.xlsx
+++ b/Documents/Logs/TimeLog_EricCarlson.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9972" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9972" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="42">
   <si>
     <t>Monday</t>
   </si>
@@ -152,6 +152,12 @@
   </si>
   <si>
     <t>Creating 3D World</t>
+  </si>
+  <si>
+    <t>Creating the 3D World</t>
+  </si>
+  <si>
+    <t>Week Total</t>
   </si>
 </sst>
 </file>
@@ -1912,7 +1918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
@@ -2180,10 +2186,359 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D26"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40">
+        <f>SUM(D28,D22,D16,D10,D4)</f>
+        <v>21.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A28:C28"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2214,290 +2569,161 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="A3" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="2" t="s">
+      <c r="A4" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="2" t="s">
+    <row r="7" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="2" t="s">
+    <row r="12" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="2" t="s">
+    <row r="16" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="2" t="s">
+    <row r="20" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="2" t="s">
+    <row r="24" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="3" t="s">
+    <row r="28" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A5:C5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
3D world completely integrated.
</commit_message>
<xml_diff>
--- a/Documents/Logs/TimeLog_EricCarlson.xlsx
+++ b/Documents/Logs/TimeLog_EricCarlson.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="43">
   <si>
     <t>Monday</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t>Week Total</t>
+  </si>
+  <si>
+    <t>Implementing the 3D World</t>
   </si>
 </sst>
 </file>
@@ -2188,8 +2191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:D28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2535,17 +2538,17 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2576,7 +2579,7 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -2590,139 +2593,192 @@
         <v>0.625</v>
       </c>
       <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C10" t="s">
         <v>40</v>
       </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="D10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="2" t="s">
+    <row r="14" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="2" t="s">
+    <row r="21" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="2" t="s">
+    <row r="27" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="2" t="s">
+    <row r="33" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" s="3" t="s">
+    <row r="39" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A5:C5"/>
+  <mergeCells count="2">
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Creating the USB Relay Interface. (not yet complete)
</commit_message>
<xml_diff>
--- a/Documents/Logs/TimeLog_EricCarlson.xlsx
+++ b/Documents/Logs/TimeLog_EricCarlson.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="46">
   <si>
     <t>Monday</t>
   </si>
@@ -161,6 +161,15 @@
   </si>
   <si>
     <t>Implementing the 3D World</t>
+  </si>
+  <si>
+    <t>Moving the Virtual Car</t>
+  </si>
+  <si>
+    <t>Research on USB Relay API</t>
+  </si>
+  <si>
+    <t>Creating USB Relay Interface</t>
   </si>
 </sst>
 </file>
@@ -2541,14 +2550,14 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2650,7 +2659,7 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -2664,76 +2673,104 @@
         <v>0.625</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="1">
+        <v>0.9375</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="B13" s="1">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="2" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="2" t="s">
+    <row r="17" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="2" t="s">
+    <row r="23" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="3" t="s">
+    <row r="29" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2778,7 +2815,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A14:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Restricted Directions based on user choice when entering practice or RC car mode.
</commit_message>
<xml_diff>
--- a/Documents/Logs/TimeLog_EricCarlson.xlsx
+++ b/Documents/Logs/TimeLog_EricCarlson.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="47">
   <si>
     <t>Monday</t>
   </si>
@@ -170,6 +170,9 @@
   </si>
   <si>
     <t>Creating USB Relay Interface</t>
+  </si>
+  <si>
+    <t>Restricting Active Trained Actions</t>
   </si>
 </sst>
 </file>
@@ -2547,17 +2550,17 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2736,6 +2739,48 @@
         <v>3</v>
       </c>
     </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+    </row>
     <row r="22" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>7</v>
@@ -2755,67 +2800,104 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="2" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="2" t="s">
+    <row r="28" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="2" t="s">
+    <row r="34" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>3</v>
+    <row r="40" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
+    <mergeCell ref="A47:C47"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A25:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Completely wired up the RC Car to the computer and finished the RC Car Component of the program. "Touch ups" will be required later.
</commit_message>
<xml_diff>
--- a/Documents/Logs/TimeLog_EricCarlson.xlsx
+++ b/Documents/Logs/TimeLog_EricCarlson.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="49">
   <si>
     <t>Monday</t>
   </si>
@@ -173,6 +173,12 @@
   </si>
   <si>
     <t>Restricting Active Trained Actions</t>
+  </si>
+  <si>
+    <t>Creating RC Car Component</t>
+  </si>
+  <si>
+    <t>Wiring RC Car to Computer</t>
   </si>
 </sst>
 </file>
@@ -2552,8 +2558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2843,6 +2849,44 @@
         <v>3</v>
       </c>
     </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31">
+        <v>4</v>
+      </c>
+    </row>
     <row r="33" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>9</v>
@@ -2881,6 +2925,20 @@
         <v>3</v>
       </c>
     </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C41" t="s">
+        <v>48</v>
+      </c>
+      <c r="D41">
+        <v>3.5</v>
+      </c>
+    </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
         <v>41</v>
@@ -2888,16 +2946,17 @@
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47">
-        <v>22</v>
+        <v>29.5</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A47:C47"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A31:C31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Restructuring the 3D World
</commit_message>
<xml_diff>
--- a/Documents/Logs/TimeLog_EricCarlson.xlsx
+++ b/Documents/Logs/TimeLog_EricCarlson.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="50">
   <si>
     <t>Monday</t>
   </si>
@@ -2967,10 +2967,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3119,67 +3119,111 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="2" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="D21">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="2" t="s">
+    <row r="26" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D27">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="2" t="s">
+    <row r="33" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" s="3" t="s">
+    <row r="39" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A22:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
The 3D World is fixed!!!!!!!!!!!!!!!!! Finally! Project nearly complete.
</commit_message>
<xml_diff>
--- a/Documents/Logs/TimeLog_EricCarlson.xlsx
+++ b/Documents/Logs/TimeLog_EricCarlson.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="55">
   <si>
     <t>Monday</t>
   </si>
@@ -182,6 +182,21 @@
   </si>
   <si>
     <t>Fixing 3D World</t>
+  </si>
+  <si>
+    <t>RC Car Bug Fixing</t>
+  </si>
+  <si>
+    <t>Practicing Presentation</t>
+  </si>
+  <si>
+    <t>Logo/Presentation</t>
+  </si>
+  <si>
+    <t>Fixing 3D World: Fixed!</t>
+  </si>
+  <si>
+    <t>Week's Total</t>
   </si>
 </sst>
 </file>
@@ -2967,17 +2982,17 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3126,6 +3141,9 @@
       <c r="B21" s="1">
         <v>0.625</v>
       </c>
+      <c r="C21" t="s">
+        <v>49</v>
+      </c>
       <c r="D21">
         <v>3.5</v>
       </c>
@@ -3166,6 +3184,9 @@
       <c r="B27" s="1">
         <v>0.41666666666666669</v>
       </c>
+      <c r="C27" t="s">
+        <v>49</v>
+      </c>
       <c r="D27">
         <v>0.5</v>
       </c>
@@ -3177,8 +3198,35 @@
       <c r="B28" s="1">
         <v>0.47916666666666669</v>
       </c>
+      <c r="C28" t="s">
+        <v>49</v>
+      </c>
       <c r="D28">
         <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C29" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30">
+        <v>3.5</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
@@ -3200,30 +3248,135 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="2" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0.5625</v>
+      </c>
+      <c r="C34" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C35" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C36" t="s">
+        <v>49</v>
+      </c>
+      <c r="D36">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>3</v>
+    <row r="40" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="C41" t="s">
+        <v>52</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C42" t="s">
+        <v>53</v>
+      </c>
+      <c r="D42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45">
+        <f>SUM(D10,D17,D22,D30,D37,D43)</f>
+        <v>21.5</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="7">
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="A45:C45"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A37:C37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
More Polishing. Log Update
</commit_message>
<xml_diff>
--- a/Documents/Logs/TimeLog_EricCarlson.xlsx
+++ b/Documents/Logs/TimeLog_EricCarlson.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9972" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9972" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="56">
   <si>
     <t>Monday</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t>Week's Total</t>
+  </si>
+  <si>
+    <t>Polishing</t>
   </si>
 </sst>
 </file>
@@ -1531,7 +1534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
@@ -1957,7 +1960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
@@ -2227,7 +2230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="A14" sqref="A14:D16"/>
     </sheetView>
   </sheetViews>
@@ -2984,7 +2987,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+    <sheetView topLeftCell="A39" workbookViewId="0">
       <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
@@ -3384,17 +3387,17 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3418,124 +3421,134 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="A3" s="1">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="2" t="s">
+    <row r="7" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="2" t="s">
+    <row r="11" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="2" t="s">
+    <row r="15" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="2" t="s">
+    <row r="19" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="2" t="s">
+    <row r="23" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="3" t="s">
+    <row r="27" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>